<commit_message>
Training classified on all training samples, saving model results
</commit_message>
<xml_diff>
--- a/final_project/shreyas/timings.xlsx
+++ b/final_project/shreyas/timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfre\Code\jupyter\cs230_spring2020\final_project\shreyas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5496A3-40A5-4BDF-A731-D67B58A206EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD434A1-85BA-4907-92B5-182601483DBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{0811D145-990C-4832-8119-159715B74B2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0811D145-990C-4832-8119-159715B74B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>1590899449.700608</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>1590943357.8945868</t>
+  </si>
+  <si>
+    <t>1590984652.9147887</t>
+  </si>
+  <si>
+    <t>1590984770.601893</t>
+  </si>
+  <si>
+    <t>on vast.ai machine with Pool() (having 16 cores)</t>
+  </si>
+  <si>
+    <t>there is another machine with 48 cores</t>
   </si>
 </sst>
 </file>
@@ -96,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,10 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3D31B3-046F-4205-81EA-D7DF3FBFBF87}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +598,37 @@
         <v>13</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <f>A18-A17</f>
+        <v>117.68711018562317</v>
+      </c>
+      <c r="C18" s="2">
+        <f>B18/60</f>
+        <v>1.9614518364270528</v>
+      </c>
+      <c r="D18" s="3">
+        <f>310000/1000*C18/60</f>
+        <v>10.134167821539773</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>